<commit_message>
fixed issue with 0 ADTV
</commit_message>
<xml_diff>
--- a/src/app/examples/processed_sample2_ptf.xlsx
+++ b/src/app/examples/processed_sample2_ptf.xlsx
@@ -517,13 +517,13 @@
         <v>1092</v>
       </c>
       <c r="C2" t="n">
-        <v>34.89</v>
+        <v>34.84</v>
       </c>
       <c r="D2" t="n">
-        <v>695853</v>
+        <v>691737</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2100092608596543</v>
+        <v>0.200459709970345</v>
       </c>
       <c r="G2" s="7" t="inlineStr">
         <is>
@@ -544,13 +544,13 @@
         <v>432</v>
       </c>
       <c r="C3" t="n">
-        <v>73.91</v>
+        <v>73.66</v>
       </c>
       <c r="D3" t="n">
-        <v>87038</v>
+        <v>89881</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1585362389066283</v>
+        <v>0.1563302702407023</v>
       </c>
     </row>
     <row r="4" ht="14.4" customHeight="1">
@@ -563,13 +563,13 @@
         <v>50</v>
       </c>
       <c r="C4" t="n">
-        <v>1292.05</v>
+        <v>1296.59</v>
       </c>
       <c r="D4" s="6" t="n">
-        <v>18084</v>
+        <v>18912</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4585911876624161</v>
+        <v>0.4882997222866197</v>
       </c>
       <c r="G4" s="9" t="inlineStr">
         <is>
@@ -587,13 +587,13 @@
         <v>238120</v>
       </c>
       <c r="C5" t="n">
-        <v>103.41</v>
+        <v>103.13</v>
       </c>
       <c r="D5" t="n">
-        <v>63234</v>
+        <v>64367</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2045415953611243</v>
+        <v>0.2025903436990393</v>
       </c>
     </row>
     <row r="6" ht="14.4" customHeight="1">
@@ -606,13 +606,13 @@
         <v>100920</v>
       </c>
       <c r="C6" t="n">
-        <v>86.5</v>
+        <v>86.34</v>
       </c>
       <c r="D6" t="n">
-        <v>3566651</v>
+        <v>3444314</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1881642177770108</v>
+        <v>0.1802370915375292</v>
       </c>
     </row>
     <row r="7">
@@ -625,13 +625,13 @@
         <v>5000</v>
       </c>
       <c r="C7" t="n">
-        <v>482.7</v>
+        <v>480.66</v>
       </c>
       <c r="D7" t="n">
-        <v>341807</v>
+        <v>364870</v>
       </c>
       <c r="E7" t="n">
-        <v>0.08663022205907903</v>
+        <v>0.1541333210277314</v>
       </c>
     </row>
     <row r="8">
@@ -644,13 +644,13 @@
         <v>1500</v>
       </c>
       <c r="C8" t="n">
-        <v>94.54000000000001</v>
+        <v>94.47</v>
       </c>
       <c r="D8" t="n">
-        <v>3999666</v>
+        <v>3949377</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1215873670099396</v>
+        <v>0.1221163772216723</v>
       </c>
     </row>
     <row r="9">
@@ -663,13 +663,13 @@
         <v>40000</v>
       </c>
       <c r="C9" t="n">
-        <v>228.76</v>
+        <v>227.87</v>
       </c>
       <c r="D9" t="n">
-        <v>1630951</v>
+        <v>1609479</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2117224709831653</v>
+        <v>0.2033037717085315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>